<commit_message>
Update proportions plot with prediction for Project 2
</commit_message>
<xml_diff>
--- a/project2/Data/weeklyincome_gender_race_1979to2018.xlsx
+++ b/project2/Data/weeklyincome_gender_race_1979to2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coverney\Documents\GitHub\ThinkStats2\project2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvu\Documents\GitHub\Cassandra\ThinkStats2\project2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2383D417-519D-40D1-B449-129E29D88AF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLS Data Series" sheetId="1" r:id="rId1"/>
@@ -21,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
-    <t>Series ID</t>
-  </si>
-  <si>
     <t>Annual
 1979</t>
   </si>
@@ -184,25 +182,28 @@
 2018</t>
   </si>
   <si>
-    <t>LEU0252883900</t>
-  </si>
-  <si>
-    <t>LEU0252884200</t>
-  </si>
-  <si>
-    <t>LEU0252885100</t>
-  </si>
-  <si>
-    <t>LEU0254468600</t>
-  </si>
-  <si>
-    <t>LEU0252886000</t>
+    <t>Asian Women</t>
+  </si>
+  <si>
+    <t>Hispanic Women</t>
+  </si>
+  <si>
+    <t>White Men</t>
+  </si>
+  <si>
+    <t>White Women</t>
+  </si>
+  <si>
+    <t>Black Women</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
@@ -221,21 +222,24 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -272,19 +276,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,14 +573,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,695 +590,695 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2">
         <v>298</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>320</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>350</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>375</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>387</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>401</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>418</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="2">
         <v>433</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="2">
         <v>450</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="2">
         <v>465</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>482</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2">
         <v>494</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="2">
         <v>506</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="2">
         <v>514</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="2">
         <v>524</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="2">
         <v>547</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="2">
         <v>566</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="2">
         <v>580</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T2" s="2">
         <v>595</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="2">
         <v>615</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="2">
         <v>638</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="2">
         <v>662</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="2">
         <v>689</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="2">
         <v>702</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="2">
         <v>715</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="2">
         <v>732</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="2">
         <v>743</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AC2" s="2">
         <v>761</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AD2" s="2">
         <v>788</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="2">
         <v>825</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AF2" s="2">
         <v>845</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AG2" s="2">
         <v>850</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AH2" s="2">
         <v>856</v>
       </c>
-      <c r="AI2" s="4">
+      <c r="AI2" s="2">
         <v>879</v>
       </c>
-      <c r="AJ2" s="4">
+      <c r="AJ2" s="2">
         <v>884</v>
       </c>
-      <c r="AK2" s="4">
+      <c r="AK2" s="2">
         <v>897</v>
       </c>
-      <c r="AL2" s="4">
+      <c r="AL2" s="2">
         <v>920</v>
       </c>
-      <c r="AM2" s="4">
+      <c r="AM2" s="2">
         <v>942</v>
       </c>
-      <c r="AN2" s="4">
+      <c r="AN2" s="2">
         <v>971</v>
       </c>
-      <c r="AO2" s="4">
+      <c r="AO2" s="2">
         <v>1002</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2">
         <v>184</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>203</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>221</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>242</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>254</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <v>268</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <v>281</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>294</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="2">
         <v>307</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="2">
         <v>318</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="2">
         <v>334</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="2">
         <v>353</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="2">
         <v>373</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="2">
         <v>387</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="2">
         <v>401</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="2">
         <v>408</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="2">
         <v>415</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="2">
         <v>428</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="2">
         <v>444</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="2">
         <v>468</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="2">
         <v>483</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W3" s="2">
         <v>502</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X3" s="2">
         <v>522</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="2">
         <v>547</v>
       </c>
-      <c r="Z3" s="4">
+      <c r="Z3" s="2">
         <v>567</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AA3" s="2">
         <v>584</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="AB3" s="2">
         <v>596</v>
       </c>
-      <c r="AC3" s="4">
+      <c r="AC3" s="2">
         <v>609</v>
       </c>
-      <c r="AD3" s="4">
+      <c r="AD3" s="2">
         <v>626</v>
       </c>
-      <c r="AE3" s="4">
+      <c r="AE3" s="2">
         <v>654</v>
       </c>
-      <c r="AF3" s="4">
+      <c r="AF3" s="2">
         <v>669</v>
       </c>
-      <c r="AG3" s="4">
+      <c r="AG3" s="2">
         <v>684</v>
       </c>
-      <c r="AH3" s="4">
+      <c r="AH3" s="2">
         <v>703</v>
       </c>
-      <c r="AI3" s="4">
+      <c r="AI3" s="2">
         <v>710</v>
       </c>
-      <c r="AJ3" s="4">
+      <c r="AJ3" s="2">
         <v>722</v>
       </c>
-      <c r="AK3" s="4">
+      <c r="AK3" s="2">
         <v>734</v>
       </c>
-      <c r="AL3" s="4">
+      <c r="AL3" s="2">
         <v>743</v>
       </c>
-      <c r="AM3" s="4">
+      <c r="AM3" s="2">
         <v>766</v>
       </c>
-      <c r="AN3" s="4">
+      <c r="AN3" s="2">
         <v>795</v>
       </c>
-      <c r="AO3" s="4">
+      <c r="AO3" s="2">
         <v>817</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2">
         <v>169</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>185</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>206</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>217</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>232</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <v>241</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>252</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>264</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="2">
         <v>276</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="2">
         <v>288</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <v>301</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="2">
         <v>308</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="2">
         <v>323</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="2">
         <v>335</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="2">
         <v>348</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="2">
         <v>346</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="2">
         <v>355</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="2">
         <v>362</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="2">
         <v>375</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="2">
         <v>400</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="2">
         <v>409</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="2">
         <v>429</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="2">
         <v>454</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y4" s="2">
         <v>473</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z4" s="2">
         <v>491</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA4" s="2">
         <v>505</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB4" s="2">
         <v>499</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC4" s="2">
         <v>519</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD4" s="2">
         <v>533</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE4" s="2">
         <v>554</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AF4" s="2">
         <v>582</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AG4" s="2">
         <v>592</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AH4" s="2">
         <v>595</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AI4" s="2">
         <v>599</v>
       </c>
-      <c r="AJ4" s="4">
+      <c r="AJ4" s="2">
         <v>606</v>
       </c>
-      <c r="AK4" s="4">
+      <c r="AK4" s="2">
         <v>611</v>
       </c>
-      <c r="AL4" s="4">
+      <c r="AL4" s="2">
         <v>615</v>
       </c>
-      <c r="AM4" s="4">
+      <c r="AM4" s="2">
         <v>641</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AN4" s="2">
         <v>657</v>
       </c>
-      <c r="AO4" s="4">
+      <c r="AO4" s="2">
         <v>654</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="W5" s="4">
+        <v>40</v>
+      </c>
+      <c r="W5" s="2">
         <v>547</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5" s="2">
         <v>563</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="2">
         <v>566</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z5" s="2">
         <v>598</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AA5" s="2">
         <v>613</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AB5" s="2">
         <v>665</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AC5" s="2">
         <v>699</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AD5" s="2">
         <v>731</v>
       </c>
-      <c r="AE5" s="4">
+      <c r="AE5" s="2">
         <v>753</v>
       </c>
-      <c r="AF5" s="4">
+      <c r="AF5" s="2">
         <v>779</v>
       </c>
-      <c r="AG5" s="4">
+      <c r="AG5" s="2">
         <v>773</v>
       </c>
-      <c r="AH5" s="4">
+      <c r="AH5" s="2">
         <v>751</v>
       </c>
-      <c r="AI5" s="4">
+      <c r="AI5" s="2">
         <v>770</v>
       </c>
-      <c r="AJ5" s="4">
+      <c r="AJ5" s="2">
         <v>819</v>
       </c>
-      <c r="AK5" s="4">
+      <c r="AK5" s="2">
         <v>841</v>
       </c>
-      <c r="AL5" s="4">
+      <c r="AL5" s="2">
         <v>877</v>
       </c>
-      <c r="AM5" s="4">
+      <c r="AM5" s="2">
         <v>902</v>
       </c>
-      <c r="AN5" s="4">
+      <c r="AN5" s="2">
         <v>903</v>
       </c>
-      <c r="AO5" s="4">
+      <c r="AO5" s="2">
         <v>937</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2">
         <v>157</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>172</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>190</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>203</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>215</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <v>223</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <v>230</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>241</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="2">
         <v>251</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="2">
         <v>260</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="2">
         <v>269</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="2">
         <v>278</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="2">
         <v>292</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="2">
         <v>302</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="2">
         <v>313</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="2">
         <v>305</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="2">
         <v>305</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="2">
         <v>316</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="2">
         <v>318</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="2">
         <v>337</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="2">
         <v>348</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6" s="2">
         <v>366</v>
       </c>
-      <c r="X6" s="4">
+      <c r="X6" s="2">
         <v>388</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="2">
         <v>397</v>
       </c>
-      <c r="Z6" s="4">
+      <c r="Z6" s="2">
         <v>410</v>
       </c>
-      <c r="AA6" s="4">
+      <c r="AA6" s="2">
         <v>419</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="AB6" s="2">
         <v>429</v>
       </c>
-      <c r="AC6" s="4">
+      <c r="AC6" s="2">
         <v>440</v>
       </c>
-      <c r="AD6" s="4">
+      <c r="AD6" s="2">
         <v>473</v>
       </c>
-      <c r="AE6" s="4">
+      <c r="AE6" s="2">
         <v>501</v>
       </c>
-      <c r="AF6" s="4">
+      <c r="AF6" s="2">
         <v>509</v>
       </c>
-      <c r="AG6" s="4">
+      <c r="AG6" s="2">
         <v>508</v>
       </c>
-      <c r="AH6" s="4">
+      <c r="AH6" s="2">
         <v>518</v>
       </c>
-      <c r="AI6" s="4">
+      <c r="AI6" s="2">
         <v>521</v>
       </c>
-      <c r="AJ6" s="4">
+      <c r="AJ6" s="2">
         <v>541</v>
       </c>
-      <c r="AK6" s="4">
+      <c r="AK6" s="2">
         <v>548</v>
       </c>
-      <c r="AL6" s="4">
+      <c r="AL6" s="2">
         <v>566</v>
       </c>
-      <c r="AM6" s="4">
+      <c r="AM6" s="2">
         <v>586</v>
       </c>
-      <c r="AN6" s="4">
+      <c r="AN6" s="2">
         <v>603</v>
       </c>
-      <c r="AO6" s="4">
+      <c r="AO6" s="2">
         <v>617</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CBureau of Labor Statistics</oddHeader>
     <oddFooter>&amp;LSource: Bureau of Labor Statistics&amp;RGenerated on: March 28, 2019 (11:06:58 PM)</oddFooter>

</xml_diff>

<commit_message>
Added plots to occupation time analysis
</commit_message>
<xml_diff>
--- a/project2/Data/weeklyincome_gender_race_1979to2018.xlsx
+++ b/project2/Data/weeklyincome_gender_race_1979to2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvu\Documents\GitHub\Cassandra\ThinkStats2\project2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coverney\Documents\GitHub\ThinkStats2\project2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2383D417-519D-40D1-B449-129E29D88AF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9074C618-3590-4A20-AE69-8739936E189E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Annual
 1979</t>
@@ -198,6 +198,36 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Black Men</t>
+  </si>
+  <si>
+    <t>Asian Men</t>
+  </si>
+  <si>
+    <t>Hispanic Men</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -207,7 +237,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -241,6 +271,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -273,8 +310,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -295,8 +333,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -574,13 +613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO6"/>
+  <dimension ref="A1:AO16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,564 +755,1688 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2">
-        <v>298</v>
+        <v>184</v>
       </c>
       <c r="C2" s="2">
-        <v>320</v>
+        <v>203</v>
       </c>
       <c r="D2" s="2">
-        <v>350</v>
+        <v>221</v>
       </c>
       <c r="E2" s="2">
-        <v>375</v>
+        <v>242</v>
       </c>
       <c r="F2" s="2">
+        <v>254</v>
+      </c>
+      <c r="G2" s="2">
+        <v>268</v>
+      </c>
+      <c r="H2" s="2">
+        <v>281</v>
+      </c>
+      <c r="I2" s="2">
+        <v>294</v>
+      </c>
+      <c r="J2" s="2">
+        <v>307</v>
+      </c>
+      <c r="K2" s="2">
+        <v>318</v>
+      </c>
+      <c r="L2" s="2">
+        <v>334</v>
+      </c>
+      <c r="M2" s="2">
+        <v>353</v>
+      </c>
+      <c r="N2" s="2">
+        <v>373</v>
+      </c>
+      <c r="O2" s="2">
         <v>387</v>
       </c>
-      <c r="G2" s="2">
+      <c r="P2" s="2">
         <v>401</v>
       </c>
-      <c r="H2" s="2">
-        <v>418</v>
-      </c>
-      <c r="I2" s="2">
-        <v>433</v>
-      </c>
-      <c r="J2" s="2">
-        <v>450</v>
-      </c>
-      <c r="K2" s="2">
-        <v>465</v>
-      </c>
-      <c r="L2" s="2">
-        <v>482</v>
-      </c>
-      <c r="M2" s="2">
-        <v>494</v>
-      </c>
-      <c r="N2" s="2">
-        <v>506</v>
-      </c>
-      <c r="O2" s="2">
-        <v>514</v>
-      </c>
-      <c r="P2" s="2">
-        <v>524</v>
-      </c>
       <c r="Q2" s="2">
+        <v>408</v>
+      </c>
+      <c r="R2" s="2">
+        <v>415</v>
+      </c>
+      <c r="S2" s="2">
+        <v>428</v>
+      </c>
+      <c r="T2" s="2">
+        <v>444</v>
+      </c>
+      <c r="U2" s="2">
+        <v>468</v>
+      </c>
+      <c r="V2" s="2">
+        <v>483</v>
+      </c>
+      <c r="W2" s="2">
+        <v>502</v>
+      </c>
+      <c r="X2" s="2">
+        <v>522</v>
+      </c>
+      <c r="Y2" s="2">
         <v>547</v>
       </c>
-      <c r="R2" s="2">
-        <v>566</v>
-      </c>
-      <c r="S2" s="2">
-        <v>580</v>
-      </c>
-      <c r="T2" s="2">
-        <v>595</v>
-      </c>
-      <c r="U2" s="2">
-        <v>615</v>
-      </c>
-      <c r="V2" s="2">
-        <v>638</v>
-      </c>
-      <c r="W2" s="2">
-        <v>662</v>
-      </c>
-      <c r="X2" s="2">
-        <v>689</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>702</v>
-      </c>
       <c r="Z2" s="2">
-        <v>715</v>
+        <v>567</v>
       </c>
       <c r="AA2" s="2">
-        <v>732</v>
+        <v>584</v>
       </c>
       <c r="AB2" s="2">
+        <v>596</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>609</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>626</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>654</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>669</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>684</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>703</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>710</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>722</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>734</v>
+      </c>
+      <c r="AL2" s="2">
         <v>743</v>
       </c>
-      <c r="AC2" s="2">
-        <v>761</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>788</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>825</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>845</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>850</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>856</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>879</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>884</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>897</v>
-      </c>
-      <c r="AL2" s="2">
-        <v>920</v>
-      </c>
       <c r="AM2" s="2">
-        <v>942</v>
+        <v>766</v>
       </c>
       <c r="AN2" s="2">
-        <v>971</v>
+        <v>795</v>
       </c>
       <c r="AO2" s="2">
-        <v>1002</v>
+        <v>817</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>43</v>
+      <c r="A3" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="2">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C3" s="2">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="D3" s="2">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E3" s="2">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="F3" s="2">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="G3" s="2">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="H3" s="2">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="I3" s="2">
-        <v>294</v>
+        <v>264</v>
       </c>
       <c r="J3" s="2">
-        <v>307</v>
+        <v>276</v>
       </c>
       <c r="K3" s="2">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="L3" s="2">
-        <v>334</v>
+        <v>301</v>
       </c>
       <c r="M3" s="2">
-        <v>353</v>
+        <v>308</v>
       </c>
       <c r="N3" s="2">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="O3" s="2">
-        <v>387</v>
+        <v>335</v>
       </c>
       <c r="P3" s="2">
-        <v>401</v>
+        <v>348</v>
       </c>
       <c r="Q3" s="2">
-        <v>408</v>
+        <v>346</v>
       </c>
       <c r="R3" s="2">
-        <v>415</v>
+        <v>355</v>
       </c>
       <c r="S3" s="2">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="T3" s="2">
-        <v>444</v>
+        <v>375</v>
       </c>
       <c r="U3" s="2">
-        <v>468</v>
+        <v>400</v>
       </c>
       <c r="V3" s="2">
-        <v>483</v>
+        <v>409</v>
       </c>
       <c r="W3" s="2">
-        <v>502</v>
+        <v>429</v>
       </c>
       <c r="X3" s="2">
-        <v>522</v>
+        <v>454</v>
       </c>
       <c r="Y3" s="2">
-        <v>547</v>
+        <v>473</v>
       </c>
       <c r="Z3" s="2">
-        <v>567</v>
+        <v>491</v>
       </c>
       <c r="AA3" s="2">
-        <v>584</v>
+        <v>505</v>
       </c>
       <c r="AB3" s="2">
-        <v>596</v>
+        <v>499</v>
       </c>
       <c r="AC3" s="2">
-        <v>609</v>
+        <v>519</v>
       </c>
       <c r="AD3" s="2">
-        <v>626</v>
+        <v>533</v>
       </c>
       <c r="AE3" s="2">
+        <v>554</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>582</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>592</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>595</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>599</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>606</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>611</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>615</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>641</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>657</v>
+      </c>
+      <c r="AO3" s="2">
         <v>654</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>669</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>684</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>703</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>710</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>722</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>734</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>743</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>766</v>
-      </c>
-      <c r="AN3" s="2">
-        <v>795</v>
-      </c>
-      <c r="AO3" s="2">
-        <v>817</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="2">
-        <v>169</v>
-      </c>
-      <c r="C4" s="2">
-        <v>185</v>
-      </c>
-      <c r="D4" s="2">
-        <v>206</v>
-      </c>
-      <c r="E4" s="2">
-        <v>217</v>
-      </c>
-      <c r="F4" s="2">
-        <v>232</v>
-      </c>
-      <c r="G4" s="2">
-        <v>241</v>
-      </c>
-      <c r="H4" s="2">
-        <v>252</v>
-      </c>
-      <c r="I4" s="2">
-        <v>264</v>
-      </c>
-      <c r="J4" s="2">
-        <v>276</v>
-      </c>
-      <c r="K4" s="2">
-        <v>288</v>
-      </c>
-      <c r="L4" s="2">
-        <v>301</v>
-      </c>
-      <c r="M4" s="2">
-        <v>308</v>
-      </c>
-      <c r="N4" s="2">
-        <v>323</v>
-      </c>
-      <c r="O4" s="2">
-        <v>335</v>
-      </c>
-      <c r="P4" s="2">
-        <v>348</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>346</v>
-      </c>
-      <c r="R4" s="2">
-        <v>355</v>
-      </c>
-      <c r="S4" s="2">
-        <v>362</v>
-      </c>
-      <c r="T4" s="2">
-        <v>375</v>
-      </c>
-      <c r="U4" s="2">
-        <v>400</v>
-      </c>
-      <c r="V4" s="2">
-        <v>409</v>
+      <c r="A4" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="W4" s="2">
-        <v>429</v>
+        <v>547</v>
       </c>
       <c r="X4" s="2">
-        <v>454</v>
+        <v>563</v>
       </c>
       <c r="Y4" s="2">
-        <v>473</v>
+        <v>566</v>
       </c>
       <c r="Z4" s="2">
-        <v>491</v>
+        <v>598</v>
       </c>
       <c r="AA4" s="2">
-        <v>505</v>
+        <v>613</v>
       </c>
       <c r="AB4" s="2">
-        <v>499</v>
+        <v>665</v>
       </c>
       <c r="AC4" s="2">
-        <v>519</v>
+        <v>699</v>
       </c>
       <c r="AD4" s="2">
-        <v>533</v>
+        <v>731</v>
       </c>
       <c r="AE4" s="2">
-        <v>554</v>
+        <v>753</v>
       </c>
       <c r="AF4" s="2">
-        <v>582</v>
+        <v>779</v>
       </c>
       <c r="AG4" s="2">
-        <v>592</v>
+        <v>773</v>
       </c>
       <c r="AH4" s="2">
-        <v>595</v>
+        <v>751</v>
       </c>
       <c r="AI4" s="2">
-        <v>599</v>
+        <v>770</v>
       </c>
       <c r="AJ4" s="2">
-        <v>606</v>
+        <v>819</v>
       </c>
       <c r="AK4" s="2">
-        <v>611</v>
+        <v>841</v>
       </c>
       <c r="AL4" s="2">
-        <v>615</v>
+        <v>877</v>
       </c>
       <c r="AM4" s="2">
-        <v>641</v>
+        <v>902</v>
       </c>
       <c r="AN4" s="2">
-        <v>657</v>
+        <v>903</v>
       </c>
       <c r="AO4" s="2">
-        <v>654</v>
+        <v>937</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
+      <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2">
+        <v>157</v>
+      </c>
+      <c r="C5" s="2">
+        <v>172</v>
+      </c>
+      <c r="D5" s="2">
+        <v>190</v>
+      </c>
+      <c r="E5" s="2">
+        <v>203</v>
+      </c>
+      <c r="F5" s="2">
+        <v>215</v>
+      </c>
+      <c r="G5" s="2">
+        <v>223</v>
+      </c>
+      <c r="H5" s="2">
+        <v>230</v>
+      </c>
+      <c r="I5" s="2">
+        <v>241</v>
+      </c>
+      <c r="J5" s="2">
+        <v>251</v>
+      </c>
+      <c r="K5" s="2">
+        <v>260</v>
+      </c>
+      <c r="L5" s="2">
+        <v>269</v>
+      </c>
+      <c r="M5" s="2">
+        <v>278</v>
+      </c>
+      <c r="N5" s="2">
+        <v>292</v>
+      </c>
+      <c r="O5" s="2">
+        <v>302</v>
+      </c>
+      <c r="P5" s="2">
+        <v>313</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>305</v>
+      </c>
+      <c r="R5" s="2">
+        <v>305</v>
+      </c>
+      <c r="S5" s="2">
+        <v>316</v>
+      </c>
+      <c r="T5" s="2">
+        <v>318</v>
+      </c>
+      <c r="U5" s="2">
+        <v>337</v>
+      </c>
+      <c r="V5" s="2">
+        <v>348</v>
       </c>
       <c r="W5" s="2">
-        <v>547</v>
+        <v>366</v>
       </c>
       <c r="X5" s="2">
-        <v>563</v>
+        <v>388</v>
       </c>
       <c r="Y5" s="2">
+        <v>397</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>410</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>419</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>429</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>440</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>473</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>501</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>509</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>508</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>518</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>521</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>541</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>548</v>
+      </c>
+      <c r="AL5" s="2">
         <v>566</v>
       </c>
-      <c r="Z5" s="2">
-        <v>598</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>613</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>665</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>699</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>731</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>753</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>779</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>773</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>751</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>770</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>819</v>
-      </c>
-      <c r="AK5" s="2">
-        <v>841</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>877</v>
-      </c>
       <c r="AM5" s="2">
-        <v>902</v>
+        <v>586</v>
       </c>
       <c r="AN5" s="2">
-        <v>903</v>
+        <v>603</v>
       </c>
       <c r="AO5" s="2">
-        <v>937</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>157</v>
+        <v>298</v>
       </c>
       <c r="C6" s="2">
-        <v>172</v>
+        <v>320</v>
       </c>
       <c r="D6" s="2">
-        <v>190</v>
+        <v>350</v>
       </c>
       <c r="E6" s="2">
-        <v>203</v>
+        <v>375</v>
       </c>
       <c r="F6" s="2">
-        <v>215</v>
+        <v>387</v>
       </c>
       <c r="G6" s="2">
+        <v>401</v>
+      </c>
+      <c r="H6" s="2">
+        <v>418</v>
+      </c>
+      <c r="I6" s="2">
+        <v>433</v>
+      </c>
+      <c r="J6" s="2">
+        <v>450</v>
+      </c>
+      <c r="K6" s="2">
+        <v>465</v>
+      </c>
+      <c r="L6" s="2">
+        <v>482</v>
+      </c>
+      <c r="M6" s="2">
+        <v>494</v>
+      </c>
+      <c r="N6" s="2">
+        <v>506</v>
+      </c>
+      <c r="O6" s="2">
+        <v>514</v>
+      </c>
+      <c r="P6" s="2">
+        <v>524</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>547</v>
+      </c>
+      <c r="R6" s="2">
+        <v>566</v>
+      </c>
+      <c r="S6" s="2">
+        <v>580</v>
+      </c>
+      <c r="T6" s="2">
+        <v>595</v>
+      </c>
+      <c r="U6" s="2">
+        <v>615</v>
+      </c>
+      <c r="V6" s="2">
+        <v>638</v>
+      </c>
+      <c r="W6" s="2">
+        <v>662</v>
+      </c>
+      <c r="X6" s="2">
+        <v>689</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>702</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>715</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>732</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>743</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>761</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>788</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>825</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>845</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>850</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>856</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>879</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>884</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>897</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>920</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>942</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>971</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2">
+        <v>227</v>
+      </c>
+      <c r="C7" s="2">
+        <v>244</v>
+      </c>
+      <c r="D7" s="2">
+        <v>268</v>
+      </c>
+      <c r="E7" s="2">
+        <v>278</v>
+      </c>
+      <c r="F7" s="2">
+        <v>294</v>
+      </c>
+      <c r="G7" s="2">
+        <v>303</v>
+      </c>
+      <c r="H7" s="2">
+        <v>305</v>
+      </c>
+      <c r="I7" s="2">
+        <v>319</v>
+      </c>
+      <c r="J7" s="2">
+        <v>327</v>
+      </c>
+      <c r="K7" s="2">
+        <v>348</v>
+      </c>
+      <c r="L7" s="2">
+        <v>348</v>
+      </c>
+      <c r="M7" s="2">
+        <v>361</v>
+      </c>
+      <c r="N7" s="2">
+        <v>375</v>
+      </c>
+      <c r="O7" s="2">
+        <v>380</v>
+      </c>
+      <c r="P7" s="2">
+        <v>392</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>400</v>
+      </c>
+      <c r="R7" s="2">
+        <v>411</v>
+      </c>
+      <c r="S7" s="2">
+        <v>412</v>
+      </c>
+      <c r="T7" s="2">
+        <v>432</v>
+      </c>
+      <c r="U7" s="2">
+        <v>468</v>
+      </c>
+      <c r="V7" s="2">
+        <v>488</v>
+      </c>
+      <c r="W7" s="2">
+        <v>510</v>
+      </c>
+      <c r="X7" s="2">
+        <v>529</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>524</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>555</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>569</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>559</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>591</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>600</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>620</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>621</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>633</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>653</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>665</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>664</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>680</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>680</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>718</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>710</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W8" s="2">
+        <v>685</v>
+      </c>
+      <c r="X8" s="2">
+        <v>732</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>756</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>772</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>802</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>825</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>882</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>936</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>966</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>952</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>936</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>970</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>1055</v>
+      </c>
+      <c r="AJ8" s="2">
+        <v>1059</v>
+      </c>
+      <c r="AK8" s="2">
+        <v>1080</v>
+      </c>
+      <c r="AL8" s="2">
+        <v>1129</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>1151</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>1207</v>
+      </c>
+      <c r="AO8" s="2">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="2">
+        <v>219</v>
+      </c>
+      <c r="C9" s="2">
+        <v>234</v>
+      </c>
+      <c r="D9" s="2">
+        <v>251</v>
+      </c>
+      <c r="E9" s="2">
+        <v>269</v>
+      </c>
+      <c r="F9" s="2">
+        <v>274</v>
+      </c>
+      <c r="G9" s="2">
+        <v>287</v>
+      </c>
+      <c r="H9" s="2">
+        <v>296</v>
+      </c>
+      <c r="I9" s="2">
+        <v>299</v>
+      </c>
+      <c r="J9" s="2">
+        <v>306</v>
+      </c>
+      <c r="K9" s="2">
+        <v>308</v>
+      </c>
+      <c r="L9" s="2">
+        <v>315</v>
+      </c>
+      <c r="M9" s="2">
+        <v>318</v>
+      </c>
+      <c r="N9" s="2">
+        <v>323</v>
+      </c>
+      <c r="O9" s="2">
+        <v>339</v>
+      </c>
+      <c r="P9" s="2">
+        <v>346</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>343</v>
+      </c>
+      <c r="R9" s="2">
+        <v>350</v>
+      </c>
+      <c r="S9" s="2">
+        <v>356</v>
+      </c>
+      <c r="T9" s="2">
+        <v>371</v>
+      </c>
+      <c r="U9" s="2">
+        <v>390</v>
+      </c>
+      <c r="V9" s="2">
+        <v>406</v>
+      </c>
+      <c r="W9" s="2">
+        <v>417</v>
+      </c>
+      <c r="X9" s="2">
+        <v>440</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>451</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>464</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>480</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>489</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>505</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>520</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>559</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>569</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>560</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>571</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>592</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>594</v>
+      </c>
+      <c r="AK9" s="2">
+        <v>616</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>631</v>
+      </c>
+      <c r="AM9" s="2">
+        <v>663</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>690</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2">
+        <v>248</v>
+      </c>
+      <c r="C10" s="2">
+        <v>269</v>
+      </c>
+      <c r="D10" s="2">
+        <v>291</v>
+      </c>
+      <c r="E10" s="2">
+        <v>310</v>
+      </c>
+      <c r="F10" s="2">
+        <v>320</v>
+      </c>
+      <c r="G10" s="2">
+        <v>336</v>
+      </c>
+      <c r="H10" s="2">
+        <v>356</v>
+      </c>
+      <c r="I10" s="2">
+        <v>371</v>
+      </c>
+      <c r="J10" s="2">
+        <v>384</v>
+      </c>
+      <c r="K10" s="2">
+        <v>395</v>
+      </c>
+      <c r="L10" s="2">
+        <v>409</v>
+      </c>
+      <c r="M10" s="2">
+        <v>424</v>
+      </c>
+      <c r="N10" s="2">
+        <v>442</v>
+      </c>
+      <c r="O10" s="2">
+        <v>458</v>
+      </c>
+      <c r="P10" s="2">
+        <v>475</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>484</v>
+      </c>
+      <c r="R10" s="2">
+        <v>494</v>
+      </c>
+      <c r="S10" s="2">
+        <v>506</v>
+      </c>
+      <c r="T10" s="2">
+        <v>519</v>
+      </c>
+      <c r="U10" s="2">
+        <v>545</v>
+      </c>
+      <c r="V10" s="2">
+        <v>573</v>
+      </c>
+      <c r="W10" s="2">
+        <v>590</v>
+      </c>
+      <c r="X10" s="2">
+        <v>610</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>623</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>636</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>657</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>672</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>690</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>716</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>742</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>757</v>
+      </c>
+      <c r="AG10" s="2">
+        <v>765</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>775</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>792</v>
+      </c>
+      <c r="AJ10" s="2">
+        <v>802</v>
+      </c>
+      <c r="AK10" s="2">
+        <v>816</v>
+      </c>
+      <c r="AL10" s="2">
+        <v>835</v>
+      </c>
+      <c r="AM10" s="2">
+        <v>862</v>
+      </c>
+      <c r="AN10" s="2">
+        <v>890</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2">
+        <v>199</v>
+      </c>
+      <c r="C11" s="2">
+        <v>212</v>
+      </c>
+      <c r="D11" s="2">
+        <v>235</v>
+      </c>
+      <c r="E11" s="2">
+        <v>245</v>
+      </c>
+      <c r="F11" s="2">
+        <v>261</v>
+      </c>
+      <c r="G11" s="2">
+        <v>269</v>
+      </c>
+      <c r="H11" s="2">
+        <v>277</v>
+      </c>
+      <c r="I11" s="2">
+        <v>291</v>
+      </c>
+      <c r="J11" s="2">
+        <v>301</v>
+      </c>
+      <c r="K11" s="2">
+        <v>314</v>
+      </c>
+      <c r="L11" s="2">
+        <v>319</v>
+      </c>
+      <c r="M11" s="2">
+        <v>329</v>
+      </c>
+      <c r="N11" s="2">
+        <v>348</v>
+      </c>
+      <c r="O11" s="2">
+        <v>357</v>
+      </c>
+      <c r="P11" s="2">
+        <v>369</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>371</v>
+      </c>
+      <c r="R11" s="2">
+        <v>383</v>
+      </c>
+      <c r="S11" s="2">
+        <v>387</v>
+      </c>
+      <c r="T11" s="2">
+        <v>400</v>
+      </c>
+      <c r="U11" s="2">
+        <v>426</v>
+      </c>
+      <c r="V11" s="2">
+        <v>445</v>
+      </c>
+      <c r="W11" s="2">
+        <v>474</v>
+      </c>
+      <c r="X11" s="2">
+        <v>491</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>498</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>514</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>525</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>520</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>554</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>569</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>589</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>601</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>611</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>615</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>621</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>629</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>639</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>641</v>
+      </c>
+      <c r="AM11" s="2">
+        <v>678</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>682</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W12" s="2">
+        <v>615</v>
+      </c>
+      <c r="X12" s="2">
+        <v>639</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>658</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>693</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>708</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>753</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>784</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>830</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>861</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>880</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>855</v>
+      </c>
+      <c r="AH12" s="2">
+        <v>866</v>
+      </c>
+      <c r="AI12" s="2">
+        <v>920</v>
+      </c>
+      <c r="AJ12" s="2">
+        <v>942</v>
+      </c>
+      <c r="AK12" s="2">
+        <v>953</v>
+      </c>
+      <c r="AL12" s="2">
+        <v>993</v>
+      </c>
+      <c r="AM12" s="2">
+        <v>1021</v>
+      </c>
+      <c r="AN12" s="2">
+        <v>1043</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2">
+        <v>194</v>
+      </c>
+      <c r="C13" s="2">
+        <v>209</v>
+      </c>
+      <c r="D13" s="2">
         <v>223</v>
       </c>
-      <c r="H6" s="2">
-        <v>230</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="E13" s="2">
+        <v>240</v>
+      </c>
+      <c r="F13" s="2">
+        <v>250</v>
+      </c>
+      <c r="G13" s="2">
+        <v>259</v>
+      </c>
+      <c r="H13" s="2">
+        <v>270</v>
+      </c>
+      <c r="I13" s="2">
+        <v>277</v>
+      </c>
+      <c r="J13" s="2">
+        <v>285</v>
+      </c>
+      <c r="K13" s="2">
+        <v>290</v>
+      </c>
+      <c r="L13" s="2">
+        <v>298</v>
+      </c>
+      <c r="M13" s="2">
+        <v>304</v>
+      </c>
+      <c r="N13" s="2">
+        <v>312</v>
+      </c>
+      <c r="O13" s="2">
+        <v>321</v>
+      </c>
+      <c r="P13" s="2">
+        <v>331</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>324</v>
+      </c>
+      <c r="R13" s="2">
+        <v>329</v>
+      </c>
+      <c r="S13" s="2">
+        <v>339</v>
+      </c>
+      <c r="T13" s="2">
+        <v>351</v>
+      </c>
+      <c r="U13" s="2">
+        <v>370</v>
+      </c>
+      <c r="V13" s="2">
+        <v>385</v>
+      </c>
+      <c r="W13" s="2">
+        <v>399</v>
+      </c>
+      <c r="X13" s="2">
+        <v>417</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>424</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>440</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>456</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>471</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>486</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>503</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>529</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>541</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>535</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>549</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>568</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>578</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>594</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>604</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>624</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>655</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2">
+        <v>182</v>
+      </c>
+      <c r="C14" s="2">
+        <v>201</v>
+      </c>
+      <c r="D14" s="2">
+        <v>219</v>
+      </c>
+      <c r="E14" s="2">
+        <v>239</v>
+      </c>
+      <c r="F14" s="2">
+        <v>252</v>
+      </c>
+      <c r="G14" s="2">
+        <v>265</v>
+      </c>
+      <c r="H14" s="2">
+        <v>277</v>
+      </c>
+      <c r="I14" s="2">
+        <v>291</v>
+      </c>
+      <c r="J14" s="2">
+        <v>303</v>
+      </c>
+      <c r="K14" s="2">
+        <v>315</v>
+      </c>
+      <c r="L14" s="2">
+        <v>328</v>
+      </c>
+      <c r="M14" s="2">
+        <v>346</v>
+      </c>
+      <c r="N14" s="2">
+        <v>366</v>
+      </c>
+      <c r="O14" s="2">
+        <v>380</v>
+      </c>
+      <c r="P14" s="2">
+        <v>393</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>399</v>
+      </c>
+      <c r="R14" s="2">
+        <v>406</v>
+      </c>
+      <c r="S14" s="2">
+        <v>418</v>
+      </c>
+      <c r="T14" s="2">
+        <v>431</v>
+      </c>
+      <c r="U14" s="2">
+        <v>456</v>
+      </c>
+      <c r="V14" s="2">
+        <v>473</v>
+      </c>
+      <c r="W14" s="2">
+        <v>493</v>
+      </c>
+      <c r="X14" s="2">
+        <v>512</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>529</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>552</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>573</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>585</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>600</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>614</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>638</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>657</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>669</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>684</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>691</v>
+      </c>
+      <c r="AJ14" s="2">
+        <v>706</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>719</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>726</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>749</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>770</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2">
+        <v>292</v>
+      </c>
+      <c r="C15" s="2">
+        <v>313</v>
+      </c>
+      <c r="D15" s="2">
+        <v>340</v>
+      </c>
+      <c r="E15" s="2">
+        <v>364</v>
+      </c>
+      <c r="F15" s="2">
+        <v>379</v>
+      </c>
+      <c r="G15" s="2">
+        <v>392</v>
+      </c>
+      <c r="H15" s="2">
+        <v>407</v>
+      </c>
+      <c r="I15" s="2">
+        <v>419</v>
+      </c>
+      <c r="J15" s="2">
+        <v>434</v>
+      </c>
+      <c r="K15" s="2">
+        <v>449</v>
+      </c>
+      <c r="L15" s="2">
+        <v>468</v>
+      </c>
+      <c r="M15" s="2">
+        <v>481</v>
+      </c>
+      <c r="N15" s="2">
+        <v>493</v>
+      </c>
+      <c r="O15" s="2">
+        <v>501</v>
+      </c>
+      <c r="P15" s="2">
+        <v>510</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>522</v>
+      </c>
+      <c r="R15" s="2">
+        <v>538</v>
+      </c>
+      <c r="S15" s="2">
+        <v>557</v>
+      </c>
+      <c r="T15" s="2">
+        <v>579</v>
+      </c>
+      <c r="U15" s="2">
+        <v>598</v>
+      </c>
+      <c r="V15" s="2">
+        <v>618</v>
+      </c>
+      <c r="W15" s="2">
+        <v>641</v>
+      </c>
+      <c r="X15" s="2">
+        <v>670</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>679</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>695</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>713</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>722</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>743</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>766</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>798</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>819</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>824</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>832</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>854</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>860</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>871</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>895</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>915</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>941</v>
+      </c>
+      <c r="AO15" s="2">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2">
         <v>241</v>
       </c>
-      <c r="J6" s="2">
-        <v>251</v>
-      </c>
-      <c r="K6" s="2">
-        <v>260</v>
-      </c>
-      <c r="L6" s="2">
-        <v>269</v>
-      </c>
-      <c r="M6" s="2">
-        <v>278</v>
-      </c>
-      <c r="N6" s="2">
-        <v>292</v>
-      </c>
-      <c r="O6" s="2">
+      <c r="C16" s="2">
+        <v>262</v>
+      </c>
+      <c r="D16" s="2">
+        <v>284</v>
+      </c>
+      <c r="E16" s="2">
         <v>302</v>
       </c>
-      <c r="P6" s="2">
+      <c r="F16" s="2">
         <v>313</v>
       </c>
-      <c r="Q6" s="2">
-        <v>305</v>
-      </c>
-      <c r="R6" s="2">
-        <v>305</v>
-      </c>
-      <c r="S6" s="2">
-        <v>316</v>
-      </c>
-      <c r="T6" s="2">
-        <v>318</v>
-      </c>
-      <c r="U6" s="2">
-        <v>337</v>
-      </c>
-      <c r="V6" s="2">
-        <v>348</v>
-      </c>
-      <c r="W6" s="2">
-        <v>366</v>
-      </c>
-      <c r="X6" s="2">
-        <v>388</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>397</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>410</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>419</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>429</v>
-      </c>
-      <c r="AC6" s="2">
+      <c r="G16" s="2">
+        <v>326</v>
+      </c>
+      <c r="H16" s="2">
+        <v>344</v>
+      </c>
+      <c r="I16" s="2">
+        <v>359</v>
+      </c>
+      <c r="J16" s="2">
+        <v>374</v>
+      </c>
+      <c r="K16" s="2">
+        <v>385</v>
+      </c>
+      <c r="L16" s="2">
+        <v>399</v>
+      </c>
+      <c r="M16" s="2">
+        <v>412</v>
+      </c>
+      <c r="N16" s="2">
+        <v>426</v>
+      </c>
+      <c r="O16" s="2">
         <v>440</v>
       </c>
-      <c r="AD6" s="2">
-        <v>473</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>501</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>509</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>508</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>518</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>521</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>541</v>
-      </c>
-      <c r="AK6" s="2">
-        <v>548</v>
-      </c>
-      <c r="AL6" s="2">
-        <v>566</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>586</v>
-      </c>
-      <c r="AN6" s="2">
-        <v>603</v>
-      </c>
-      <c r="AO6" s="2">
-        <v>617</v>
+      <c r="P16" s="2">
+        <v>459</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>467</v>
+      </c>
+      <c r="R16" s="2">
+        <v>479</v>
+      </c>
+      <c r="S16" s="2">
+        <v>490</v>
+      </c>
+      <c r="T16" s="2">
+        <v>503</v>
+      </c>
+      <c r="U16" s="2">
+        <v>523</v>
+      </c>
+      <c r="V16" s="2">
+        <v>549</v>
+      </c>
+      <c r="W16" s="2">
+        <v>576</v>
+      </c>
+      <c r="X16" s="2">
+        <v>596</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>608</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>620</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>638</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>651</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>671</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>695</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>722</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>739</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>747</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>756</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>768</v>
+      </c>
+      <c r="AJ16" s="2">
+        <v>776</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>791</v>
+      </c>
+      <c r="AL16" s="2">
+        <v>809</v>
+      </c>
+      <c r="AM16" s="2">
+        <v>832</v>
+      </c>
+      <c r="AN16" s="2">
+        <v>860</v>
+      </c>
+      <c r="AO16" s="2">
+        <v>886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>